<commit_message>
Kodutoo2 esimesed 4 osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B113C9E-D928-4C0A-9DB1-7FAC079FABFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A78D627-E3C3-4B0E-AD3E-57F6EE7C4214}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3516" yWindow="3156" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Praktikum GitHub kasutamise kohta</t>
+  </si>
+  <si>
+    <t>Kodutöö Razor pages</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,15 +1116,29 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5">
+        <v>200</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
@@ -1231,7 +1248,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>530</v>
+        <v>730</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Kodutoo tehtud ja exceli uuendus
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643423B1-3D80-4260-88F4-72A9D5D83E5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF083F8C-2D46-4B74-B805-479EDAEBD50D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Kodutöö Razor pages</t>
+  </si>
+  <si>
+    <t>HTML ja CSS õppimine + konspekt</t>
   </si>
 </sst>
 </file>
@@ -894,7 +897,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,40 +1175,80 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="7">
+        <v>43868</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5">
+        <v>90</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="10"/>
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="7">
+        <v>43868</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.9375</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5">
+        <v>60</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="7">
+        <v>43869</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1214,29 +1257,59 @@
       <c r="A16" s="9">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="7">
+        <v>43869</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5">
+        <v>80</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="B17" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5">
+        <v>70</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
@@ -1262,7 +1335,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>860</v>
+        <v>1220</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Alustasin kodutoo 17 veebruar, tegin esimesed 5
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF5FD43-F241-42B7-85C4-5EEE6B96B71F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F2AE41-3D79-4A6C-B395-C33EE92FEC89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Teise kodutöö konspekti täiendamine</t>
+  </si>
+  <si>
+    <t>Kodutoo MVC</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="43">
-        <v>43871</v>
+        <v>43878</v>
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
@@ -1103,29 +1106,59 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="7">
+        <v>43873</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.9375</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="7">
+        <v>43876</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5">
+        <v>170</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
@@ -1235,7 +1268,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>180</v>
+        <v>410</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
kodutoo MVC + excel
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F2AE41-3D79-4A6C-B395-C33EE92FEC89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CCB24-8BA6-4D8E-B558-7813BFFFA269}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -910,7 +910,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,29 +1164,59 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="5">
+        <v>60</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5">
+        <v>230</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="10"/>
+      <c r="I13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
@@ -1268,7 +1298,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>410</v>
+        <v>700</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Lopetasin kodutoo + excel
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CCB24-8BA6-4D8E-B558-7813BFFFA269}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE2837-8CC3-4456-BCB6-23BB48AB4047}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -910,7 +910,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,13 +1113,13 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="D10" s="8">
-        <v>0.9375</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>29</v>
@@ -1168,7 +1168,7 @@
         <v>43877</v>
       </c>
       <c r="C12" s="8">
-        <v>0.57638888888888895</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="D12" s="8">
         <v>0.61805555555555558</v>
@@ -1177,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="5">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>32</v>
@@ -1199,13 +1199,13 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D13" s="8">
-        <v>0.8125</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>32</v>
@@ -1298,7 +1298,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Parandasin ühe vea Person classis
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE2837-8CC3-4456-BCB6-23BB48AB4047}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA883D67-C531-49EC-98CA-4B400292A553}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Kodutoo MVC</t>
+  </si>
+  <si>
+    <t>Kodutoo MVC+konspekti korrastus</t>
   </si>
 </sst>
 </file>
@@ -910,7 +913,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,40 +1214,68 @@
         <v>32</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="I13" s="6"/>
       <c r="J13" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="7">
+        <v>43878</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="E14" s="6">
+        <v>80</v>
+      </c>
+      <c r="F14" s="5">
+        <v>190</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="7">
+        <v>43878</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
@@ -1298,7 +1329,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>790</v>
+        <v>1040</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
logi uuendus (uus nadal)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA883D67-C531-49EC-98CA-4B400292A553}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0A397D-7557-416E-8988-58BA08007797}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 3" sheetId="4" r:id="rId1"/>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Nädal 4" sheetId="5" r:id="rId1"/>
+    <sheet name="Nädal 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="34">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -909,10 +910,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98AD9E4-5B33-4A6F-A57A-6A6C2C428068}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="43">
+        <v>43885</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43879</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="21">
+        <v>90</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>90</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6BF5AF-5009-4F6E-A844-B08EEF064221}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BB784D-1582-4652-B455-CD642B6FE3D6}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -1816,7 +2142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>

</xml_diff>

<commit_message>
17 veebruar kodutoo exception parandus
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0A397D-7557-416E-8988-58BA08007797}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969FE515-89C3-42F0-BAEE-9FC2BD7074D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Kodutoo MVC+konspekti korrastus</t>
+  </si>
+  <si>
+    <t>Praktikum breakpoint ja debuggimine</t>
   </si>
 </sst>
 </file>
@@ -914,7 +917,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,14 +1055,28 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="7">
+        <v>43880</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5">
+        <v>60</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1212,7 +1229,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
exceli uuendus, 6 videot tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gluzk\source\repos\KodutoodProgemine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0B0E3A-29ED-4B9C-B6C3-75E7D5F46087}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435752C8-778D-4E87-A7B3-D69EB3B1DE62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Teine ja kolmas videoloeng</t>
+  </si>
+  <si>
+    <t>Alustasin neljanda  videoga</t>
+  </si>
+  <si>
+    <t>Esimesed 6 videot tehtud</t>
   </si>
 </sst>
 </file>
@@ -926,7 +932,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,12 +1156,24 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="7">
+        <v>43883</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5">
+        <v>60</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1164,15 +1182,31 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="7">
+        <v>43884</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.9375</v>
+      </c>
+      <c r="E12" s="6">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5">
+        <v>200</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -1268,7 +1302,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>660</v>
+        <v>920</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>